<commit_message>
Account creation mapped to data sheet
</commit_message>
<xml_diff>
--- a/testdata/PolicyCenter.xlsx
+++ b/testdata/PolicyCenter.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\asrikanth\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C66938-C894-4FED-AACD-67F677EAF709}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01834AC-90F2-41DF-936E-9FD1159F3B8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="15000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="8" r:id="rId1"/>
     <sheet name="Coverage" sheetId="7" r:id="rId2"/>
     <sheet name="Login" sheetId="1" r:id="rId3"/>
-    <sheet name="AccountCreation" sheetId="2" r:id="rId4"/>
-    <sheet name="Policy" sheetId="3" r:id="rId5"/>
-    <sheet name="AcctSummary" sheetId="5" r:id="rId6"/>
+    <sheet name="createAccount" sheetId="2" r:id="rId4"/>
+    <sheet name="organizations" sheetId="9" r:id="rId5"/>
+    <sheet name="Policy" sheetId="3" r:id="rId6"/>
+    <sheet name="AcctSummary" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="296">
   <si>
     <t>TD_UserName</t>
   </si>
@@ -116,15 +117,6 @@
     <t>TD_CompanyName</t>
   </si>
   <si>
-    <t>QA1BILLINGPLAN01</t>
-  </si>
-  <si>
-    <t>BillPlan1</t>
-  </si>
-  <si>
-    <t>BillPlan2</t>
-  </si>
-  <si>
     <t>BillPlan3</t>
   </si>
   <si>
@@ -134,18 +126,9 @@
     <t>BillPlan5</t>
   </si>
   <si>
-    <t>Insured</t>
-  </si>
-  <si>
-    <t>Equity-Based Delinquency Plan</t>
-  </si>
-  <si>
     <t>Wright Construction</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Direct Bill</t>
   </si>
   <si>
@@ -791,57 +774,12 @@
     <t>AUT_TS_118</t>
   </si>
   <si>
-    <t>Account No</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Office Phone</t>
-  </si>
-  <si>
     <t>Fax</t>
   </si>
   <si>
-    <t>Home Phone</t>
-  </si>
-  <si>
-    <t>Work Phone</t>
-  </si>
-  <si>
-    <t>Mobile Phone</t>
-  </si>
-  <si>
-    <t>Fax Phone</t>
-  </si>
-  <si>
-    <t>Primary Phone</t>
-  </si>
-  <si>
-    <t>Primary Email</t>
-  </si>
-  <si>
-    <t>Secondary Email</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>Address 2</t>
-  </si>
-  <si>
-    <t>Address 3</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -851,15 +789,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>ZIP Code</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">NB_ModProg_AddintionalInsured Add </t>
   </si>
   <si>
@@ -870,6 +799,126 @@
   </si>
   <si>
     <t>&gt; Secondary Named Insured Add &gt; UW Company Mod &gt; Driver Info Add &gt; Vehicle Info Add &gt; Coverages Modification &gt; Prior policies Entry &gt; Billing Type 1 &gt; 6 months schedule &gt; Premium match&gt;Policy Details Review&gt;Forms trigger and ordering validation&gt;Billing type &gt; PC &gt; Secondary Named Insured Del"</t>
+  </si>
+  <si>
+    <t>OfficePhone</t>
+  </si>
+  <si>
+    <t>HomePhone</t>
+  </si>
+  <si>
+    <t>WorkPhone</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>FaxPhone</t>
+  </si>
+  <si>
+    <t>PrimaryPhone</t>
+  </si>
+  <si>
+    <t>PrimaryEmail</t>
+  </si>
+  <si>
+    <t>SecondaryEmail</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>ZIPCode</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PersonalAccount1</t>
+  </si>
+  <si>
+    <t>CompanyAccount1</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>South Avenue</t>
+  </si>
+  <si>
+    <t>DownTown</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>AddressType</t>
+  </si>
+  <si>
+    <t>AccountNickname</t>
+  </si>
+  <si>
+    <t>OrganizationName</t>
+  </si>
+  <si>
+    <t>OrganizationType</t>
+  </si>
+  <si>
+    <t>Organization1</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Search_Button</t>
+  </si>
+  <si>
+    <t>Reset_Button</t>
+  </si>
+  <si>
+    <t>ProducerTier</t>
+  </si>
+  <si>
+    <t>ProducerCode</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>ACV Property Insurance</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>301-008578</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>OfficialID</t>
   </si>
 </sst>
 </file>
@@ -1293,39 +1342,39 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E2" s="15">
         <v>44286</v>
@@ -1335,21 +1384,21 @@
       </c>
       <c r="G2" s="7"/>
       <c r="I2" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E3" s="15">
         <v>44286</v>
@@ -1361,16 +1410,16 @@
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E4" s="15">
         <v>44286</v>
@@ -1382,16 +1431,16 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E5" s="15">
         <v>44286</v>
@@ -1403,13 +1452,13 @@
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1418,11 +1467,11 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1431,11 +1480,11 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1444,11 +1493,11 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1457,11 +1506,11 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1470,11 +1519,11 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1483,11 +1532,11 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1496,11 +1545,11 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1509,11 +1558,11 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1522,11 +1571,11 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1535,11 +1584,11 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1548,11 +1597,11 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1561,11 +1610,11 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1574,11 +1623,11 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1587,11 +1636,11 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1600,11 +1649,11 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1613,11 +1662,11 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1626,11 +1675,11 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1639,11 +1688,11 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1652,11 +1701,11 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1665,11 +1714,11 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1678,11 +1727,11 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1691,11 +1740,11 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1704,11 +1753,11 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -1717,11 +1766,11 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -1730,11 +1779,11 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1743,11 +1792,11 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1756,11 +1805,11 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1769,11 +1818,11 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -1782,11 +1831,11 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1795,11 +1844,11 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1808,11 +1857,11 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1821,11 +1870,11 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -1834,11 +1883,11 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -1847,11 +1896,11 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -1860,11 +1909,11 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -1873,11 +1922,11 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -1886,11 +1935,11 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B43" s="14"/>
       <c r="C43" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -1899,11 +1948,11 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -1912,11 +1961,11 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -1925,11 +1974,11 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -1938,11 +1987,11 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B47" s="14"/>
       <c r="C47" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -1951,11 +2000,11 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -1964,11 +2013,11 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -1977,11 +2026,11 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -1990,11 +2039,11 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B51" s="14"/>
       <c r="C51" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
@@ -2003,11 +2052,11 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
@@ -2016,11 +2065,11 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -2029,11 +2078,11 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -2042,11 +2091,11 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2055,11 +2104,11 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
@@ -2068,11 +2117,11 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -2081,11 +2130,11 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B58" s="14"/>
       <c r="C58" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -2094,11 +2143,11 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B59" s="14"/>
       <c r="C59" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
@@ -2107,11 +2156,11 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
@@ -2120,11 +2169,11 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
@@ -2133,11 +2182,11 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B62" s="14"/>
       <c r="C62" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
@@ -2146,11 +2195,11 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -2159,11 +2208,11 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
@@ -2172,11 +2221,11 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B65" s="14"/>
       <c r="C65" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -2185,11 +2234,11 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B66" s="14"/>
       <c r="C66" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -2198,11 +2247,11 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
@@ -2211,11 +2260,11 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -2224,11 +2273,11 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B69" s="14"/>
       <c r="C69" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
@@ -2237,11 +2286,11 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B70" s="14"/>
       <c r="C70" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
@@ -2250,11 +2299,11 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B71" s="14"/>
       <c r="C71" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -2263,11 +2312,11 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -2276,11 +2325,11 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -2289,11 +2338,11 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
@@ -2302,11 +2351,11 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
@@ -2315,11 +2364,11 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B76" s="14"/>
       <c r="C76" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
@@ -2328,11 +2377,11 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B77" s="14"/>
       <c r="C77" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
@@ -2341,11 +2390,11 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B78" s="14"/>
       <c r="C78" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
@@ -2354,11 +2403,11 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
@@ -2367,11 +2416,11 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B80" s="14"/>
       <c r="C80" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
@@ -2380,11 +2429,11 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B81" s="14"/>
       <c r="C81" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
@@ -2393,11 +2442,11 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B82" s="14"/>
       <c r="C82" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
@@ -2406,11 +2455,11 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -2419,11 +2468,11 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -2432,11 +2481,11 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B85" s="14"/>
       <c r="C85" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -2445,11 +2494,11 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -2458,11 +2507,11 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
@@ -2471,11 +2520,11 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
@@ -2484,11 +2533,11 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
@@ -2497,11 +2546,11 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -2510,11 +2559,11 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B91" s="14"/>
       <c r="C91" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
@@ -2523,11 +2572,11 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B92" s="14"/>
       <c r="C92" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
@@ -2536,11 +2585,11 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B93" s="14"/>
       <c r="C93" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -2549,11 +2598,11 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
@@ -2562,11 +2611,11 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B95" s="14"/>
       <c r="C95" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
@@ -2575,11 +2624,11 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B96" s="14"/>
       <c r="C96" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
@@ -2588,11 +2637,11 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B97" s="14"/>
       <c r="C97" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
@@ -2601,11 +2650,11 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B98" s="14"/>
       <c r="C98" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
@@ -2614,11 +2663,11 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B99" s="14"/>
       <c r="C99" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
@@ -2627,11 +2676,11 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B100" s="14"/>
       <c r="C100" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
@@ -2640,11 +2689,11 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B101" s="14"/>
       <c r="C101" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
@@ -2653,11 +2702,11 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B102" s="14"/>
       <c r="C102" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
@@ -2666,11 +2715,11 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B103" s="14"/>
       <c r="C103" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
@@ -2679,11 +2728,11 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B104" s="14"/>
       <c r="C104" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
@@ -2692,11 +2741,11 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B105" s="14"/>
       <c r="C105" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
@@ -2705,11 +2754,11 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -2718,11 +2767,11 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
@@ -2731,11 +2780,11 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B108" s="14"/>
       <c r="C108" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -2744,11 +2793,11 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B109" s="14"/>
       <c r="C109" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
@@ -2757,11 +2806,11 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
@@ -2770,11 +2819,11 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B111" s="14"/>
       <c r="C111" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
@@ -2783,11 +2832,11 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B112" s="14"/>
       <c r="C112" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
@@ -2796,11 +2845,11 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B113" s="14"/>
       <c r="C113" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
@@ -2809,11 +2858,11 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B114" s="14"/>
       <c r="C114" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
@@ -2822,11 +2871,11 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B115" s="14"/>
       <c r="C115" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -2835,11 +2884,11 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B116" s="14"/>
       <c r="C116" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -2848,11 +2897,11 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B117" s="14"/>
       <c r="C117" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -2861,11 +2910,11 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
@@ -2874,11 +2923,11 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
@@ -2907,909 +2956,909 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="17" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="17" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="17" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="17" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="17" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="17" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3823,7 +3872,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3940,37 +3989,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="C1" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="D1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F1" t="s">
         <v>257</v>
@@ -3994,101 +4060,125 @@
         <v>263</v>
       </c>
       <c r="M1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N1" t="s">
         <v>264</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>265</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>266</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" t="s">
+        <v>250</v>
+      </c>
+      <c r="S1" t="s">
+        <v>251</v>
+      </c>
+      <c r="T1" t="s">
         <v>267</v>
       </c>
-      <c r="Q1" t="s">
-        <v>268</v>
-      </c>
-      <c r="R1" t="s">
-        <v>269</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>279</v>
+      </c>
+      <c r="V1" t="s">
+        <v>280</v>
+      </c>
+      <c r="W1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="T1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="F2">
+        <v>2015551002</v>
+      </c>
+      <c r="G2">
+        <v>2015551003</v>
+      </c>
+      <c r="H2">
+        <v>2015551004</v>
+      </c>
+      <c r="I2">
+        <v>2015551005</v>
+      </c>
+      <c r="J2" t="s">
+        <v>274</v>
+      </c>
+      <c r="K2" t="s">
+        <v>272</v>
+      </c>
+      <c r="M2" t="s">
+        <v>275</v>
+      </c>
+      <c r="N2" t="s">
+        <v>272</v>
+      </c>
+      <c r="O2" t="s">
+        <v>276</v>
+      </c>
+      <c r="P2" t="s">
+        <v>277</v>
+      </c>
+      <c r="U2" t="s">
+        <v>278</v>
+      </c>
+      <c r="V2" t="s">
+        <v>272</v>
+      </c>
+      <c r="W2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="U1" t="s">
+      <c r="B3" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="V1" t="s">
+      <c r="C3" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="W1" t="s">
-        <v>274</v>
-      </c>
-      <c r="X1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4097,6 +4187,97 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CB62B0-3E14-40DE-9CB1-C3C158CCA48E}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I1" t="s">
+        <v>288</v>
+      </c>
+      <c r="J1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K1" t="s">
+        <v>290</v>
+      </c>
+      <c r="L1" t="s">
+        <v>285</v>
+      </c>
+      <c r="M1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2" t="s">
+        <v>293</v>
+      </c>
+      <c r="L2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B240F2F-8AD3-49E3-9150-9222387F22C2}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -4120,36 +4301,36 @@
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F2" s="8">
         <v>1000</v>
@@ -4157,7 +4338,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -4167,7 +4348,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -4177,7 +4358,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -4187,7 +4368,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
@@ -4201,11 +4382,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -4227,31 +4408,31 @@
         <v>26</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="12"/>
@@ -4260,7 +4441,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="12"/>
@@ -4269,7 +4450,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="12"/>
@@ -4278,7 +4459,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="12"/>

</xml_diff>

<commit_message>
Coverages and quotes updated
</commit_message>
<xml_diff>
--- a/testdata/PolicyCenter.xlsx
+++ b/testdata/PolicyCenter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\training2\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\training2\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC12\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A4E8CB-7FA0-4ADD-9CEE-EA8AC6C61051}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B0B038-A94A-402B-972F-80D3887B9C19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="10425" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="310">
   <si>
     <t>TD_UserName</t>
   </si>
@@ -950,7 +950,19 @@
     <t>AUT_PC_AC_05</t>
   </si>
   <si>
-    <t>Medical Limit</t>
+    <t>RentalCarLossofUseLimit</t>
+  </si>
+  <si>
+    <t>UnderinsuredMotoristPropertyDamageLimit</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>MedicalLimit</t>
   </si>
 </sst>
 </file>
@@ -4680,10 +4692,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB72CC37-2FC1-4BE3-AA8A-0E623FF584F9}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4691,9 +4703,11 @@
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4701,10 +4715,19 @@
         <v>296</v>
       </c>
       <c r="C1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>304</v>
       </c>
@@ -4713,6 +4736,15 @@
       </c>
       <c r="C2" s="19">
         <v>5000</v>
+      </c>
+      <c r="D2" s="19">
+        <v>25000</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
personal auto - excel issue
</commit_message>
<xml_diff>
--- a/testdata/PolicyCenter.xlsx
+++ b/testdata/PolicyCenter.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\achandrasekaran\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C11D36-2AEC-40F5-949C-859EE486E47D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FB386EC1-3728-4B44-9298-3710488DE5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="8" r:id="rId1"/>
@@ -23,26 +18,18 @@
     <sheet name="PA_Coverages" sheetId="10" r:id="rId8"/>
     <sheet name="DropDown_List" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="675">
   <si>
     <t>TD_UserName</t>
   </si>
@@ -2064,6 +2051,9 @@
   </si>
   <si>
     <t>AUT_PersonalAuto_PolicyCenter_Renewal__Withdraw Transaction</t>
+  </si>
+  <si>
+    <t>zxczx</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2140,11 +2130,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2195,6 +2196,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5115,10 +5122,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C375"/>
+  <dimension ref="A1:C376"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D375"/>
+      <selection activeCell="A359" sqref="A359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9250,6 +9257,17 @@
         <v>1</v>
       </c>
       <c r="C375" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>674</v>
+      </c>
+      <c r="B376" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C376" s="21" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>